<commit_message>
Update and Add File
</commit_message>
<xml_diff>
--- a/src/RegistanFerghanaLC.Web/wwwroot/files/template.xlsx
+++ b/src/RegistanFerghanaLC.Web/wwwroot/files/template.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -21,37 +21,69 @@
     <t>surname</t>
   </si>
   <si>
-    <t>phone</t>
+    <t xml:space="preserve">birthdate
+</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>part of day</t>
+  </si>
+  <si>
+    <t>work days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone
+</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>subject</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
     <t>john</t>
   </si>
   <si>
     <t>doe</t>
   </si>
   <si>
-    <t>+998336661313</t>
+    <t>23.02.2002</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Even</t>
   </si>
   <si>
     <t>Admin12345</t>
   </si>
   <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>Beginner</t>
+    <t>miya</t>
+  </si>
+  <si>
+    <t>sami</t>
+  </si>
+  <si>
+    <t>12.06.2000</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Odd</t>
+  </si>
+  <si>
+    <t>Admin3290</t>
   </si>
 </sst>
 </file>
@@ -59,10 +91,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <color rgb="FFA31515"/>
+      <sz val="9"/>
+      <name val="Cascadia Mono"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -86,16 +129,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" shrinkToFit="false" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" shrinkToFit="false" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" shrinkToFit="false" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" shrinkToFit="false" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyNumberFormat="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" shrinkToFit="false" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -108,32 +155,37 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showZeros="true" showFormulas="false" showGridLines="true" showRowColHeaders="true">
-      <selection sqref="G6" activeCell="G6"/>
+      <selection sqref="C4" activeCell="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" customHeight="true" defaultRowHeight="15"/>
   <cols>
-    <col max="3" min="1" style="0" width="12.140625"/>
-    <col max="4" min="4" style="0" width="17.99609375" customWidth="true"/>
-    <col max="5" min="5" style="0" width="15.42578125" customWidth="true"/>
-    <col max="8" min="6" style="0" width="12.140625"/>
+    <col max="3" min="1" style="1" width="12.140625" customWidth="true" bestFit="true"/>
+    <col max="4" min="4" style="1" width="17.99609375" customWidth="true"/>
+    <col max="5" min="5" style="1" width="14.85546875" customWidth="true"/>
+    <col max="7" min="6" style="1" width="12.140625" customWidth="true" bestFit="true"/>
+    <col max="8" min="8" style="1" width="17.7109375" customWidth="true"/>
+    <col max="9" min="9" style="0" width="20.28515625" customWidth="true"/>
+    <col max="10" min="10" style="0" width="21.140625" customWidth="true"/>
+    <col max="12" min="12" style="0" width="12.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -145,41 +197,94 @@
       <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>37310</v>
+      <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>998973645867</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="F4" s="2"/>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>998946576823</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5">
       <c r="F5" s="2"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="29">
+      <c r="L29" s="3"/>
     </row>
   </sheetData>
   <pageSetup orientation="default" fitToHeight="0" fitToWidth="0" cellComments="none"/>

</xml_diff>